<commit_message>
updating dictionary and function
</commit_message>
<xml_diff>
--- a/inst/extdata/mne_dictionary.xlsx
+++ b/inst/extdata/mne_dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="var_defs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="552">
   <si>
     <t>var_name</t>
   </si>
@@ -661,12 +661,6 @@
     <t>indicator_1</t>
   </si>
   <si>
-    <t>intervetnion_funding</t>
-  </si>
-  <si>
-    <t>intervetnion_funding_total</t>
-  </si>
-  <si>
     <t>indicator_2</t>
   </si>
   <si>
@@ -1547,6 +1541,141 @@
   </si>
   <si>
     <t>Veuillez indiquer le nombre total de tests effectués dans le pays au cours de la dernière semaine et préciser le nombre de tests réalisés dans des laboratoires décentralisés. En outre, veuillez expliquer dans le résumé écrit tout changement subi par ces chiffres.</t>
+  </si>
+  <si>
+    <t>intervention_funding</t>
+  </si>
+  <si>
+    <t>intervention_funding_total</t>
+  </si>
+  <si>
+    <t>Number of ntational staff in IMST</t>
+  </si>
+  <si>
+    <t>BLANK</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Adding duplicate for misspelt english version</t>
+  </si>
+  <si>
+    <t>Number of points of entry with  screening, isolation facilities and referral system for COVID-19</t>
+  </si>
+  <si>
+    <t>Number of contacts identified during the last 7 days</t>
+  </si>
+  <si>
+    <t>Total number of contacts under follow-up during the last 7 day</t>
+  </si>
+  <si>
+    <t>Total number of contacts under follow-up</t>
+  </si>
+  <si>
+    <t>Number of laboratory results made available within 48 hours for samples collected within the last two days</t>
+  </si>
+  <si>
+    <t>Performance Indicator 17: Bed occupancy rate for confirmed cases at present</t>
+  </si>
+  <si>
+    <t>Estimate of percentageof individuals reached by RCCE activity (e.g. CHW  trainings, health worker trainings, hotline usage )</t>
+  </si>
+  <si>
+    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the last month</t>
+  </si>
+  <si>
+    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the same month in 2019</t>
+  </si>
+  <si>
+    <t>Number of people living with HIV in target area who received ART in the current week</t>
+  </si>
+  <si>
+    <t>Total number of contacts under follow-up during the last 7 days</t>
+  </si>
+  <si>
+    <t>Total approved national COVID-19 response budget ($)</t>
+  </si>
+  <si>
+    <t>Amount of approved budget national budget utilized to date ($)</t>
+  </si>
+  <si>
+    <t>Total WCO response funding ($)</t>
+  </si>
+  <si>
+    <t>Amount of WCO response funding utilized to date ($)</t>
+  </si>
+  <si>
+    <t>Anticipated total IMST staff needed</t>
+  </si>
+  <si>
+    <t>Nuimber of points of entry with  screening, isolation facilities and referral system for COVID-19</t>
+  </si>
+  <si>
+    <t>Cumulative number of tests per 10 000 population performed at the end of the previous week  ( Tests-3501)</t>
+  </si>
+  <si>
+    <t>Cumulative number of tests per 10 000 population performed at the end of the current week  (Tests-2071)</t>
+  </si>
+  <si>
+    <t>Number of consultations in primary health facilities and prenatal clinics during the same month in 2019 (August)</t>
+  </si>
+  <si>
+    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the last month  (August 2020)</t>
+  </si>
+  <si>
+    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the same month (August 2019)</t>
+  </si>
+  <si>
+    <t>Number of people living with HIV in target area who received ART in the current week (Annual  total for 2020)</t>
+  </si>
+  <si>
+    <t>Number of people living with HIV in target area who received ART during the same week in 2019 (Annual total for 2019)</t>
+  </si>
+  <si>
+    <t>Cumulative number of tests per 10 000 population performed at the end of the previous week  ( Tests-1633) =1633/13785346.5</t>
+  </si>
+  <si>
+    <t>Cumulative number of tests per 10 000 population performed at the end of the current week  (Tests-2024)=2024/13785346.5</t>
+  </si>
+  <si>
+    <t>Number of consultations in primary health facilities and prenatal clinics during the last month (September 2020)</t>
+  </si>
+  <si>
+    <t>Number of consultations in primary health facilities and prenatal clinics during the same month in 2019 (September)</t>
+  </si>
+  <si>
+    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the last month  (Sept 2020)</t>
+  </si>
+  <si>
+    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the same month (Sept 2019)</t>
+  </si>
+  <si>
+    <t>Nombre de cas contacts signalés au cours des sept derniers jours</t>
+  </si>
+  <si>
+    <t>Adding duplicate for misspelt french version</t>
+  </si>
+  <si>
+    <t>Nombre de cas contacts signalés ayant fait l’objet d’une investigation dans les 24 heures au cours des sept derniers jours</t>
+  </si>
+  <si>
+    <t>Indicateur d’exécution n° 5 : Pourcentage du personnel de l’ESGI du bureau de pays déployé dans les ESGI décentralisées ou les soutenant</t>
+  </si>
+  <si>
+    <t>Indicateur d’exécution n° 15 : Taux d’occupation actuel des lits par les cas suspects (en pourcentage)</t>
+  </si>
+  <si>
+    <t>Indicateur d’exécution n° 19 : Taux de létalité</t>
+  </si>
+  <si>
+    <t>Indicateur d’exécution n° 23 : Taux de létalité des cas confirmés signalés au cours des sept derniers jours</t>
+  </si>
+  <si>
+    <t>Nombre de patients en soins ambulatoires au cours du mois dernier ( Avril)</t>
+  </si>
+  <si>
+    <t>Adding duplicate misspelt french version</t>
   </si>
 </sst>
 </file>
@@ -1898,10 +2027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C153"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C107" sqref="C5:C107"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,9 +2038,10 @@
     <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="185.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1919,10 +2049,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="D1" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -1930,10 +2063,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>208</v>
       </c>
@@ -1941,10 +2074,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -1952,10 +2085,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>210</v>
       </c>
@@ -1963,1634 +2096,2145 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" t="s">
+        <v>510</v>
+      </c>
+      <c r="C6" t="s">
+        <v>524</v>
+      </c>
+      <c r="D6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" t="s">
+        <v>510</v>
+      </c>
+      <c r="C8" t="s">
+        <v>525</v>
+      </c>
+      <c r="D8" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>211</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>507</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>212</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>507</v>
+      </c>
+      <c r="B11" t="s">
+        <v>510</v>
+      </c>
+      <c r="C11" t="s">
+        <v>526</v>
+      </c>
+      <c r="D11" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>508</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>508</v>
+      </c>
+      <c r="B13" t="s">
+        <v>510</v>
+      </c>
+      <c r="C13" t="s">
+        <v>527</v>
+      </c>
+      <c r="D13" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>213</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>214</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>215</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B17" t="s">
+        <v>510</v>
+      </c>
+      <c r="C17" t="s">
+        <v>528</v>
+      </c>
+      <c r="D17" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>216</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>217</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>217</v>
+      </c>
+      <c r="B20" t="s">
+        <v>510</v>
+      </c>
+      <c r="C20" t="s">
+        <v>509</v>
+      </c>
+      <c r="D20" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>218</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>219</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>220</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B23" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C23" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>220</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C24" t="s">
+        <v>510</v>
+      </c>
+      <c r="D24" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>221</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>222</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>223</v>
       </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>224</v>
       </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>225</v>
       </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>226</v>
       </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>227</v>
       </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>228</v>
       </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>229</v>
       </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>230</v>
       </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>231</v>
       </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36" t="s">
+        <v>510</v>
+      </c>
+      <c r="C36" t="s">
+        <v>513</v>
+      </c>
+      <c r="D36" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37" t="s">
+        <v>510</v>
+      </c>
+      <c r="C37" t="s">
+        <v>529</v>
+      </c>
+      <c r="D37" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>232</v>
       </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>233</v>
       </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B40" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>234</v>
       </c>
-      <c r="B30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>235</v>
       </c>
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>236</v>
       </c>
-      <c r="B32" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>237</v>
       </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>238</v>
       </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>239</v>
       </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>240</v>
       </c>
-      <c r="B36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>241</v>
       </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>242</v>
       </c>
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>242</v>
+      </c>
+      <c r="B50" t="s">
+        <v>543</v>
+      </c>
+      <c r="C50" t="s">
+        <v>510</v>
+      </c>
+      <c r="D50" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>243</v>
       </c>
-      <c r="B39" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C51" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>243</v>
+      </c>
+      <c r="B52" t="s">
+        <v>545</v>
+      </c>
+      <c r="C52" t="s">
+        <v>510</v>
+      </c>
+      <c r="D52" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>244</v>
       </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>245</v>
       </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B54" t="s">
+        <v>43</v>
+      </c>
+      <c r="C54" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>245</v>
+      </c>
+      <c r="B55" t="s">
+        <v>510</v>
+      </c>
+      <c r="C55" t="s">
+        <v>514</v>
+      </c>
+      <c r="D55" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>246</v>
       </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>246</v>
+      </c>
+      <c r="B57" t="s">
+        <v>510</v>
+      </c>
+      <c r="C57" t="s">
+        <v>515</v>
+      </c>
+      <c r="D57" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>246</v>
+      </c>
+      <c r="B58" t="s">
+        <v>510</v>
+      </c>
+      <c r="C58" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>247</v>
       </c>
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>247</v>
+      </c>
+      <c r="B60" t="s">
+        <v>510</v>
+      </c>
+      <c r="C60" t="s">
+        <v>516</v>
+      </c>
+      <c r="D60" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>248</v>
       </c>
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B61" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>249</v>
       </c>
-      <c r="B45" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="B62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>250</v>
       </c>
-      <c r="B46" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>251</v>
       </c>
-      <c r="B47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>251</v>
+      </c>
+      <c r="B65" t="s">
+        <v>510</v>
+      </c>
+      <c r="C65" t="s">
+        <v>517</v>
+      </c>
+      <c r="D65" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>252</v>
       </c>
-      <c r="B48" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B66" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>253</v>
       </c>
-      <c r="B49" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B67" t="s">
+        <v>51</v>
+      </c>
+      <c r="C67" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>253</v>
+      </c>
+      <c r="B68" t="s">
+        <v>510</v>
+      </c>
+      <c r="C68" t="s">
+        <v>530</v>
+      </c>
+      <c r="D68" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>253</v>
+      </c>
+      <c r="B69" t="s">
+        <v>510</v>
+      </c>
+      <c r="C69" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>254</v>
       </c>
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B70" t="s">
+        <v>52</v>
+      </c>
+      <c r="C70" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>254</v>
+      </c>
+      <c r="B71" t="s">
+        <v>510</v>
+      </c>
+      <c r="C71" t="s">
+        <v>531</v>
+      </c>
+      <c r="D71" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>254</v>
+      </c>
+      <c r="B72" t="s">
+        <v>510</v>
+      </c>
+      <c r="C72" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>255</v>
       </c>
-      <c r="B51" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B73" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>256</v>
       </c>
-      <c r="B52" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B74" t="s">
+        <v>54</v>
+      </c>
+      <c r="C74" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>257</v>
       </c>
-      <c r="B53" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B75" t="s">
+        <v>55</v>
+      </c>
+      <c r="C75" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>258</v>
       </c>
-      <c r="B54" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+      <c r="C76" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>259</v>
       </c>
-      <c r="B55" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>260</v>
       </c>
-      <c r="B56" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B78" t="s">
+        <v>58</v>
+      </c>
+      <c r="C78" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>261</v>
       </c>
-      <c r="B57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B79" t="s">
+        <v>59</v>
+      </c>
+      <c r="C79" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>262</v>
       </c>
-      <c r="B58" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B80" t="s">
+        <v>60</v>
+      </c>
+      <c r="C80" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>263</v>
       </c>
-      <c r="B59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B81" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C81" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>263</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="C82" t="s">
+        <v>510</v>
+      </c>
+      <c r="D82" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>264</v>
       </c>
-      <c r="B60" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B83" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>265</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B84" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C84" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>266</v>
       </c>
-      <c r="B62" t="s">
-        <v>61</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B85" t="s">
+        <v>62</v>
+      </c>
+      <c r="C85" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>267</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B86" t="s">
+        <v>63</v>
+      </c>
+      <c r="C86" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>268</v>
       </c>
-      <c r="B64" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B87" t="s">
+        <v>64</v>
+      </c>
+      <c r="C87" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>268</v>
+      </c>
+      <c r="B88" t="s">
+        <v>510</v>
+      </c>
+      <c r="C88" t="s">
+        <v>518</v>
+      </c>
+      <c r="D88" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>269</v>
       </c>
-      <c r="B65" t="s">
-        <v>63</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B89" t="s">
+        <v>65</v>
+      </c>
+      <c r="C89" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>270</v>
       </c>
-      <c r="B66" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B90" t="s">
+        <v>66</v>
+      </c>
+      <c r="C90" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>271</v>
       </c>
-      <c r="B67" t="s">
-        <v>65</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B91" t="s">
+        <v>67</v>
+      </c>
+      <c r="C91" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>272</v>
       </c>
-      <c r="B68" t="s">
-        <v>66</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B92" t="s">
+        <v>68</v>
+      </c>
+      <c r="C92" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>273</v>
       </c>
-      <c r="B69" t="s">
-        <v>67</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B93" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C93" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>273</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="C94" t="s">
+        <v>510</v>
+      </c>
+      <c r="D94" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>274</v>
       </c>
-      <c r="B70" t="s">
-        <v>68</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="B95" t="s">
+        <v>69</v>
+      </c>
+      <c r="C95" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>275</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B96" t="s">
+        <v>70</v>
+      </c>
+      <c r="C96" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>276</v>
       </c>
-      <c r="B72" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B97" t="s">
+        <v>71</v>
+      </c>
+      <c r="C97" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>277</v>
       </c>
-      <c r="B73" t="s">
-        <v>70</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B98" t="s">
+        <v>72</v>
+      </c>
+      <c r="C98" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>278</v>
       </c>
-      <c r="B74" t="s">
-        <v>71</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B99" t="s">
+        <v>73</v>
+      </c>
+      <c r="C99" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>279</v>
       </c>
-      <c r="B75" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="B100" t="s">
+        <v>74</v>
+      </c>
+      <c r="C100" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>280</v>
       </c>
-      <c r="B76" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="B101" t="s">
+        <v>75</v>
+      </c>
+      <c r="C101" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>281</v>
       </c>
-      <c r="B77" t="s">
-        <v>74</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="B102" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>282</v>
       </c>
-      <c r="B78" t="s">
-        <v>75</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B103" t="s">
+        <v>77</v>
+      </c>
+      <c r="C103" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>283</v>
       </c>
-      <c r="B79" t="s">
-        <v>76</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="B104" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C104" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>283</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C105" t="s">
+        <v>510</v>
+      </c>
+      <c r="D105" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>284</v>
       </c>
-      <c r="B80" t="s">
-        <v>77</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="B106" t="s">
+        <v>78</v>
+      </c>
+      <c r="C106" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>285</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="B107" t="s">
+        <v>79</v>
+      </c>
+      <c r="C107" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>286</v>
       </c>
-      <c r="B82" t="s">
-        <v>78</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="B108" t="s">
+        <v>80</v>
+      </c>
+      <c r="C108" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>287</v>
       </c>
-      <c r="B83" t="s">
-        <v>79</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="B109" t="s">
+        <v>81</v>
+      </c>
+      <c r="C109" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>288</v>
       </c>
-      <c r="B84" t="s">
-        <v>80</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="B110" t="s">
+        <v>82</v>
+      </c>
+      <c r="C110" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>289</v>
       </c>
-      <c r="B85" t="s">
-        <v>81</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="B111" t="s">
+        <v>83</v>
+      </c>
+      <c r="C111" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>290</v>
       </c>
-      <c r="B86" t="s">
-        <v>82</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B112" t="s">
+        <v>84</v>
+      </c>
+      <c r="C112" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>290</v>
+      </c>
+      <c r="B113" t="s">
+        <v>510</v>
+      </c>
+      <c r="C113" t="s">
+        <v>519</v>
+      </c>
+      <c r="D113" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>291</v>
       </c>
-      <c r="B87" t="s">
-        <v>83</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="B114" t="s">
+        <v>85</v>
+      </c>
+      <c r="C114" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>292</v>
       </c>
-      <c r="B88" t="s">
-        <v>84</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="B115" t="s">
+        <v>86</v>
+      </c>
+      <c r="C115" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>293</v>
       </c>
-      <c r="B89" t="s">
-        <v>85</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B116" t="s">
+        <v>87</v>
+      </c>
+      <c r="C116" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>294</v>
       </c>
-      <c r="B90" t="s">
-        <v>86</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="B117" t="s">
+        <v>88</v>
+      </c>
+      <c r="C117" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>295</v>
       </c>
-      <c r="B91" t="s">
-        <v>87</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="B118" t="s">
+        <v>89</v>
+      </c>
+      <c r="C118" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>295</v>
+      </c>
+      <c r="B119" t="s">
+        <v>510</v>
+      </c>
+      <c r="C119" t="s">
+        <v>539</v>
+      </c>
+      <c r="D119" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>296</v>
       </c>
-      <c r="B92" t="s">
-        <v>88</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B120" t="s">
+        <v>90</v>
+      </c>
+      <c r="C120" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>296</v>
+      </c>
+      <c r="B121" t="s">
+        <v>510</v>
+      </c>
+      <c r="C121" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>296</v>
+      </c>
+      <c r="B122" t="s">
+        <v>510</v>
+      </c>
+      <c r="C122" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>297</v>
       </c>
-      <c r="B93" t="s">
-        <v>89</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="B123" t="s">
+        <v>91</v>
+      </c>
+      <c r="C123" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>298</v>
       </c>
-      <c r="B94" t="s">
-        <v>90</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="B124" t="s">
+        <v>92</v>
+      </c>
+      <c r="C124" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>298</v>
+      </c>
+      <c r="B125" t="s">
+        <v>510</v>
+      </c>
+      <c r="C125" t="s">
+        <v>520</v>
+      </c>
+      <c r="D125" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>298</v>
+      </c>
+      <c r="B126" t="s">
+        <v>510</v>
+      </c>
+      <c r="C126" t="s">
+        <v>533</v>
+      </c>
+      <c r="D126" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>298</v>
+      </c>
+      <c r="B127" t="s">
+        <v>510</v>
+      </c>
+      <c r="C127" t="s">
+        <v>541</v>
+      </c>
+      <c r="D127" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>299</v>
       </c>
-      <c r="B95" t="s">
-        <v>91</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="B128" t="s">
+        <v>93</v>
+      </c>
+      <c r="C128" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>299</v>
+      </c>
+      <c r="B129" t="s">
+        <v>510</v>
+      </c>
+      <c r="C129" t="s">
+        <v>521</v>
+      </c>
+      <c r="D129" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>299</v>
+      </c>
+      <c r="B130" t="s">
+        <v>510</v>
+      </c>
+      <c r="C130" t="s">
+        <v>534</v>
+      </c>
+      <c r="D130" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>299</v>
+      </c>
+      <c r="B131" t="s">
+        <v>510</v>
+      </c>
+      <c r="C131" t="s">
+        <v>542</v>
+      </c>
+      <c r="D131" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>300</v>
       </c>
-      <c r="B96" t="s">
-        <v>92</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="B132" t="s">
+        <v>94</v>
+      </c>
+      <c r="C132" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>301</v>
       </c>
-      <c r="B97" t="s">
-        <v>93</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="B133" t="s">
+        <v>95</v>
+      </c>
+      <c r="C133" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>301</v>
+      </c>
+      <c r="B134" t="s">
+        <v>550</v>
+      </c>
+      <c r="C134" t="s">
+        <v>510</v>
+      </c>
+      <c r="D134" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>302</v>
       </c>
-      <c r="B98" t="s">
-        <v>94</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="B135" t="s">
+        <v>96</v>
+      </c>
+      <c r="C135" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>303</v>
       </c>
-      <c r="B99" t="s">
-        <v>95</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B136" t="s">
+        <v>97</v>
+      </c>
+      <c r="C136" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>304</v>
       </c>
-      <c r="B100" t="s">
-        <v>96</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="B137" t="s">
+        <v>98</v>
+      </c>
+      <c r="C137" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>304</v>
+      </c>
+      <c r="B138" t="s">
+        <v>510</v>
+      </c>
+      <c r="C138" t="s">
+        <v>522</v>
+      </c>
+      <c r="D138" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>304</v>
+      </c>
+      <c r="B139" t="s">
+        <v>510</v>
+      </c>
+      <c r="C139" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>305</v>
       </c>
-      <c r="B101" t="s">
-        <v>97</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="B140" t="s">
+        <v>99</v>
+      </c>
+      <c r="C140" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>305</v>
+      </c>
+      <c r="B141" t="s">
+        <v>510</v>
+      </c>
+      <c r="C141" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>306</v>
       </c>
-      <c r="B102" t="s">
-        <v>98</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="B142" t="s">
+        <v>100</v>
+      </c>
+      <c r="C142" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>307</v>
       </c>
-      <c r="B103" t="s">
-        <v>99</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="B143" t="s">
+        <v>101</v>
+      </c>
+      <c r="C143" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>308</v>
       </c>
-      <c r="B104" t="s">
-        <v>100</v>
-      </c>
-      <c r="C104" t="s">
+      <c r="B144" t="s">
+        <v>102</v>
+      </c>
+      <c r="C144" t="s">
         <v>461</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>309</v>
-      </c>
-      <c r="B105" t="s">
-        <v>101</v>
-      </c>
-      <c r="C105" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>310</v>
-      </c>
-      <c r="B106" t="s">
-        <v>102</v>
-      </c>
-      <c r="C106" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>311</v>
-      </c>
-      <c r="B107" t="s">
-        <v>103</v>
-      </c>
-      <c r="C107" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>312</v>
-      </c>
-      <c r="B108" t="s">
-        <v>104</v>
-      </c>
-      <c r="C108" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>313</v>
-      </c>
-      <c r="B109" t="s">
-        <v>105</v>
-      </c>
-      <c r="C109" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>314</v>
-      </c>
-      <c r="B110" t="s">
-        <v>106</v>
-      </c>
-      <c r="C110" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>315</v>
-      </c>
-      <c r="B111" t="s">
-        <v>107</v>
-      </c>
-      <c r="C111" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>316</v>
-      </c>
-      <c r="B112" t="s">
-        <v>108</v>
-      </c>
-      <c r="C112" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>317</v>
-      </c>
-      <c r="B113" t="s">
-        <v>109</v>
-      </c>
-      <c r="C113" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>318</v>
-      </c>
-      <c r="B114" t="s">
-        <v>110</v>
-      </c>
-      <c r="C114" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>319</v>
-      </c>
-      <c r="B115" t="s">
-        <v>111</v>
-      </c>
-      <c r="C115" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>320</v>
-      </c>
-      <c r="B116" t="s">
-        <v>112</v>
-      </c>
-      <c r="C116" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>321</v>
-      </c>
-      <c r="B117" t="s">
-        <v>113</v>
-      </c>
-      <c r="C117" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>322</v>
-      </c>
-      <c r="B118" t="s">
-        <v>114</v>
-      </c>
-      <c r="C118" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>323</v>
-      </c>
-      <c r="B119" t="s">
-        <v>115</v>
-      </c>
-      <c r="C119" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>324</v>
-      </c>
-      <c r="B120" t="s">
-        <v>116</v>
-      </c>
-      <c r="C120" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>325</v>
-      </c>
-      <c r="B121" t="s">
-        <v>117</v>
-      </c>
-      <c r="C121" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>326</v>
-      </c>
-      <c r="B122" t="s">
-        <v>118</v>
-      </c>
-      <c r="C122" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>327</v>
-      </c>
-      <c r="B123" t="s">
-        <v>119</v>
-      </c>
-      <c r="C123" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>328</v>
-      </c>
-      <c r="B124" t="s">
-        <v>120</v>
-      </c>
-      <c r="C124" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>329</v>
-      </c>
-      <c r="B125" t="s">
-        <v>121</v>
-      </c>
-      <c r="C125" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>330</v>
-      </c>
-      <c r="B126" t="s">
-        <v>122</v>
-      </c>
-      <c r="C126" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>331</v>
-      </c>
-      <c r="B127" t="s">
-        <v>123</v>
-      </c>
-      <c r="C127" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>332</v>
-      </c>
-      <c r="B128" t="s">
-        <v>124</v>
-      </c>
-      <c r="C128" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>333</v>
-      </c>
-      <c r="B129" t="s">
-        <v>125</v>
-      </c>
-      <c r="C129" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>334</v>
-      </c>
-      <c r="B130" t="s">
-        <v>126</v>
-      </c>
-      <c r="C130" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>335</v>
-      </c>
-      <c r="B131" t="s">
-        <v>127</v>
-      </c>
-      <c r="C131" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>336</v>
-      </c>
-      <c r="B132" t="s">
-        <v>128</v>
-      </c>
-      <c r="C132" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>337</v>
-      </c>
-      <c r="B133" t="s">
-        <v>129</v>
-      </c>
-      <c r="C133" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>338</v>
-      </c>
-      <c r="B134" t="s">
-        <v>130</v>
-      </c>
-      <c r="C134" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>339</v>
-      </c>
-      <c r="B135" t="s">
-        <v>131</v>
-      </c>
-      <c r="C135" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>340</v>
-      </c>
-      <c r="B136" t="s">
-        <v>132</v>
-      </c>
-      <c r="C136" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>341</v>
-      </c>
-      <c r="B137" t="s">
-        <v>133</v>
-      </c>
-      <c r="C137" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>342</v>
-      </c>
-      <c r="B138" t="s">
-        <v>134</v>
-      </c>
-      <c r="C138" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>343</v>
-      </c>
-      <c r="B139" t="s">
-        <v>135</v>
-      </c>
-      <c r="C139" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>344</v>
-      </c>
-      <c r="B140" t="s">
-        <v>136</v>
-      </c>
-      <c r="C140" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>345</v>
-      </c>
-      <c r="B141" t="s">
-        <v>137</v>
-      </c>
-      <c r="C141" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>346</v>
-      </c>
-      <c r="B142" t="s">
-        <v>138</v>
-      </c>
-      <c r="C142" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>347</v>
-      </c>
-      <c r="B143" t="s">
-        <v>139</v>
-      </c>
-      <c r="C143" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>348</v>
-      </c>
-      <c r="B144" t="s">
-        <v>140</v>
-      </c>
-      <c r="C144" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>349</v>
+        <v>309</v>
       </c>
       <c r="B145" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="C145" t="s">
-        <v>141</v>
+        <v>462</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>350</v>
+        <v>310</v>
       </c>
       <c r="B146" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="C146" t="s">
-        <v>142</v>
+        <v>463</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>351</v>
+        <v>311</v>
       </c>
       <c r="B147" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="C147" t="s">
-        <v>143</v>
+        <v>464</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>352</v>
+        <v>312</v>
       </c>
       <c r="B148" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="C148" t="s">
-        <v>144</v>
+        <v>465</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>353</v>
+        <v>313</v>
       </c>
       <c r="B149" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="C149" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>354</v>
+        <v>314</v>
       </c>
       <c r="B150" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="C150" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>355</v>
+        <v>315</v>
       </c>
       <c r="B151" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="C151" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>356</v>
+        <v>316</v>
       </c>
       <c r="B152" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="C152" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>357</v>
+        <v>317</v>
       </c>
       <c r="B153" t="s">
+        <v>111</v>
+      </c>
+      <c r="C153" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>318</v>
+      </c>
+      <c r="B154" t="s">
+        <v>112</v>
+      </c>
+      <c r="C154" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>319</v>
+      </c>
+      <c r="B155" t="s">
+        <v>113</v>
+      </c>
+      <c r="C155" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>320</v>
+      </c>
+      <c r="B156" t="s">
+        <v>114</v>
+      </c>
+      <c r="C156" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>321</v>
+      </c>
+      <c r="B157" t="s">
+        <v>115</v>
+      </c>
+      <c r="C157" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>322</v>
+      </c>
+      <c r="B158" t="s">
+        <v>116</v>
+      </c>
+      <c r="C158" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>323</v>
+      </c>
+      <c r="B159" t="s">
+        <v>117</v>
+      </c>
+      <c r="C159" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>324</v>
+      </c>
+      <c r="B160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C160" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>325</v>
+      </c>
+      <c r="B161" t="s">
+        <v>119</v>
+      </c>
+      <c r="C161" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>326</v>
+      </c>
+      <c r="B162" t="s">
+        <v>120</v>
+      </c>
+      <c r="C162" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>327</v>
+      </c>
+      <c r="B163" t="s">
+        <v>121</v>
+      </c>
+      <c r="C163" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>328</v>
+      </c>
+      <c r="B164" t="s">
+        <v>122</v>
+      </c>
+      <c r="C164" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>329</v>
+      </c>
+      <c r="B165" t="s">
+        <v>123</v>
+      </c>
+      <c r="C165" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" t="s">
+        <v>124</v>
+      </c>
+      <c r="C166" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167" t="s">
+        <v>125</v>
+      </c>
+      <c r="C167" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>332</v>
+      </c>
+      <c r="B168" t="s">
+        <v>126</v>
+      </c>
+      <c r="C168" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>333</v>
+      </c>
+      <c r="B169" t="s">
+        <v>127</v>
+      </c>
+      <c r="C169" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>334</v>
+      </c>
+      <c r="B170" t="s">
+        <v>128</v>
+      </c>
+      <c r="C170" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>335</v>
+      </c>
+      <c r="B171" t="s">
+        <v>129</v>
+      </c>
+      <c r="C171" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>336</v>
+      </c>
+      <c r="B172" t="s">
+        <v>130</v>
+      </c>
+      <c r="C172" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>337</v>
+      </c>
+      <c r="B173" t="s">
+        <v>131</v>
+      </c>
+      <c r="C173" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>338</v>
+      </c>
+      <c r="B174" t="s">
+        <v>132</v>
+      </c>
+      <c r="C174" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>339</v>
+      </c>
+      <c r="B175" t="s">
+        <v>133</v>
+      </c>
+      <c r="C175" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>340</v>
+      </c>
+      <c r="B176" t="s">
+        <v>134</v>
+      </c>
+      <c r="C176" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>341</v>
+      </c>
+      <c r="B177" t="s">
+        <v>135</v>
+      </c>
+      <c r="C177" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>342</v>
+      </c>
+      <c r="B178" t="s">
+        <v>136</v>
+      </c>
+      <c r="C178" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>343</v>
+      </c>
+      <c r="B179" t="s">
+        <v>137</v>
+      </c>
+      <c r="C179" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>344</v>
+      </c>
+      <c r="B180" t="s">
+        <v>138</v>
+      </c>
+      <c r="C180" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>345</v>
+      </c>
+      <c r="B181" t="s">
+        <v>139</v>
+      </c>
+      <c r="C181" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>346</v>
+      </c>
+      <c r="B182" t="s">
+        <v>140</v>
+      </c>
+      <c r="C182" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>347</v>
+      </c>
+      <c r="B183" t="s">
+        <v>141</v>
+      </c>
+      <c r="C183" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>348</v>
+      </c>
+      <c r="B184" t="s">
+        <v>142</v>
+      </c>
+      <c r="C184" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>349</v>
+      </c>
+      <c r="B185" t="s">
+        <v>143</v>
+      </c>
+      <c r="C185" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>350</v>
+      </c>
+      <c r="B186" t="s">
+        <v>144</v>
+      </c>
+      <c r="C186" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>351</v>
+      </c>
+      <c r="B187" t="s">
+        <v>145</v>
+      </c>
+      <c r="C187" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>352</v>
+      </c>
+      <c r="B188" t="s">
+        <v>146</v>
+      </c>
+      <c r="C188" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>353</v>
+      </c>
+      <c r="B189" t="s">
+        <v>147</v>
+      </c>
+      <c r="C189" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>354</v>
+      </c>
+      <c r="B190" t="s">
+        <v>148</v>
+      </c>
+      <c r="C190" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>355</v>
+      </c>
+      <c r="B191" t="s">
         <v>149</v>
       </c>
-      <c r="C153" t="s">
+      <c r="C191" t="s">
         <v>149</v>
       </c>
     </row>
@@ -3604,7 +4248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -3624,10 +4268,10 @@
         <v>206</v>
       </c>
       <c r="C1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3638,10 +4282,10 @@
         <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3649,7 +4293,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3657,7 +4301,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3668,10 +4312,10 @@
         <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D5" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3679,7 +4323,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3687,7 +4331,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,10 +4342,10 @@
         <v>203</v>
       </c>
       <c r="C8" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3709,7 +4353,7 @@
         <v>202</v>
       </c>
       <c r="C9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3717,7 +4361,7 @@
         <v>201</v>
       </c>
       <c r="C10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3728,10 +4372,10 @@
         <v>195</v>
       </c>
       <c r="C11" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D11" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3739,7 +4383,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3750,10 +4394,10 @@
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3761,7 +4405,7 @@
         <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3772,10 +4416,10 @@
         <v>198</v>
       </c>
       <c r="C15" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D15" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3783,7 +4427,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3794,10 +4438,10 @@
         <v>197</v>
       </c>
       <c r="C17" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D17" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,7 +4449,7 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3816,10 +4460,10 @@
         <v>196</v>
       </c>
       <c r="C19" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D19" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3827,7 +4471,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,7 +4479,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,10 +4490,10 @@
         <v>195</v>
       </c>
       <c r="C22" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D22" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3857,7 +4501,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3865,7 +4509,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3876,10 +4520,10 @@
         <v>193</v>
       </c>
       <c r="C25" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D25" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,7 +4531,7 @@
         <v>192</v>
       </c>
       <c r="C26" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3895,7 +4539,7 @@
         <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3906,10 +4550,10 @@
         <v>191</v>
       </c>
       <c r="C28" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D28" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3920,10 +4564,10 @@
         <v>190</v>
       </c>
       <c r="C29" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D29" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3934,10 +4578,10 @@
         <v>189</v>
       </c>
       <c r="C30" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D30" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3945,7 +4589,7 @@
         <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3953,7 +4597,7 @@
         <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3964,10 +4608,10 @@
         <v>187</v>
       </c>
       <c r="C33" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D33" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3978,10 +4622,10 @@
         <v>186</v>
       </c>
       <c r="C34" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D34" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3989,7 +4633,7 @@
         <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3997,7 +4641,7 @@
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -4008,10 +4652,10 @@
         <v>185</v>
       </c>
       <c r="C37" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D37" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4019,7 +4663,7 @@
         <v>41</v>
       </c>
       <c r="C38" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4027,7 +4671,7 @@
         <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4038,10 +4682,10 @@
         <v>184</v>
       </c>
       <c r="C40" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D40" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4052,10 +4696,10 @@
         <v>183</v>
       </c>
       <c r="C41" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D41" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,10 +4710,10 @@
         <v>182</v>
       </c>
       <c r="C42" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D42" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4077,7 +4721,7 @@
         <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4085,7 +4729,7 @@
         <v>180</v>
       </c>
       <c r="C44" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -4096,10 +4740,10 @@
         <v>179</v>
       </c>
       <c r="C45" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D45" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4107,7 +4751,7 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,7 +4759,7 @@
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -4126,10 +4770,10 @@
         <v>178</v>
       </c>
       <c r="C48" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D48" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4137,7 +4781,7 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -4145,7 +4789,7 @@
         <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -4153,13 +4797,13 @@
         <v>54</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C51" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D51" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -4167,13 +4811,13 @@
         <v>55</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C52" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D52" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,7 +4825,7 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -4189,7 +4833,7 @@
         <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -4200,10 +4844,10 @@
         <v>177</v>
       </c>
       <c r="C55" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D55" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -4214,10 +4858,10 @@
         <v>173</v>
       </c>
       <c r="C56" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D56" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -4225,7 +4869,7 @@
         <v>60</v>
       </c>
       <c r="C57" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -4233,7 +4877,7 @@
         <v>176</v>
       </c>
       <c r="C58" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4244,10 +4888,10 @@
         <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D59" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4255,7 +4899,7 @@
         <v>174</v>
       </c>
       <c r="C60" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4266,10 +4910,10 @@
         <v>173</v>
       </c>
       <c r="C61" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D61" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4277,7 +4921,7 @@
         <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4285,7 +4929,7 @@
         <v>64</v>
       </c>
       <c r="C63" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4296,10 +4940,10 @@
         <v>173</v>
       </c>
       <c r="C64" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D64" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4307,7 +4951,7 @@
         <v>66</v>
       </c>
       <c r="C65" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4315,7 +4959,7 @@
         <v>67</v>
       </c>
       <c r="C66" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4326,10 +4970,10 @@
         <v>171</v>
       </c>
       <c r="C67" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D67" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -4337,7 +4981,7 @@
         <v>170</v>
       </c>
       <c r="C68" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -4348,10 +4992,10 @@
         <v>169</v>
       </c>
       <c r="C69" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D69" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -4359,7 +5003,7 @@
         <v>70</v>
       </c>
       <c r="C70" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -4370,10 +5014,10 @@
         <v>168</v>
       </c>
       <c r="C71" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D71" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -4381,7 +5025,7 @@
         <v>72</v>
       </c>
       <c r="C72" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -4392,10 +5036,10 @@
         <v>167</v>
       </c>
       <c r="C73" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D73" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -4406,10 +5050,10 @@
         <v>166</v>
       </c>
       <c r="C74" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D74" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -4417,7 +5061,7 @@
         <v>165</v>
       </c>
       <c r="C75" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -4425,7 +5069,7 @@
         <v>164</v>
       </c>
       <c r="C76" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -4436,10 +5080,10 @@
         <v>163</v>
       </c>
       <c r="C77" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D77" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -4447,7 +5091,7 @@
         <v>162</v>
       </c>
       <c r="C78" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -4458,10 +5102,10 @@
         <v>161</v>
       </c>
       <c r="C79" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D79" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -4469,7 +5113,7 @@
         <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -4480,10 +5124,10 @@
         <v>160</v>
       </c>
       <c r="C81" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D81" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -4491,7 +5135,7 @@
         <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -4499,7 +5143,7 @@
         <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -4510,10 +5154,10 @@
         <v>159</v>
       </c>
       <c r="C84" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D84" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -4524,10 +5168,10 @@
         <v>157</v>
       </c>
       <c r="C85" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D85" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -4535,7 +5179,7 @@
         <v>85</v>
       </c>
       <c r="C86" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -4543,7 +5187,7 @@
         <v>86</v>
       </c>
       <c r="C87" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -4551,7 +5195,7 @@
         <v>87</v>
       </c>
       <c r="C88" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -4559,7 +5203,7 @@
         <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -4570,10 +5214,10 @@
         <v>155</v>
       </c>
       <c r="C90" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D90" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -4581,7 +5225,7 @@
         <v>90</v>
       </c>
       <c r="C91" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -4589,7 +5233,7 @@
         <v>91</v>
       </c>
       <c r="C92" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -4600,10 +5244,10 @@
         <v>152</v>
       </c>
       <c r="C93" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D93" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -4611,7 +5255,7 @@
         <v>93</v>
       </c>
       <c r="C94" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -4619,7 +5263,7 @@
         <v>94</v>
       </c>
       <c r="C95" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -4630,10 +5274,10 @@
         <v>152</v>
       </c>
       <c r="C96" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D96" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -4641,7 +5285,7 @@
         <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -4649,7 +5293,7 @@
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -4660,10 +5304,10 @@
         <v>152</v>
       </c>
       <c r="C99" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D99" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,7 +5315,7 @@
         <v>99</v>
       </c>
       <c r="C100" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -4679,7 +5323,7 @@
         <v>151</v>
       </c>
       <c r="C101" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -4690,10 +5334,10 @@
         <v>150</v>
       </c>
       <c r="C102" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D102" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -4701,7 +5345,7 @@
         <v>102</v>
       </c>
       <c r="C103" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -4709,7 +5353,7 @@
         <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finishing up long merge
</commit_message>
<xml_diff>
--- a/inst/extdata/mne_dictionary.xlsx
+++ b/inst/extdata/mne_dictionary.xlsx
@@ -9,18 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="var_defs" sheetId="1" r:id="rId1"/>
     <sheet name="comment_refs" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">var_defs!$A$1:$D$153</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="510">
   <si>
     <t>var_name</t>
   </si>
@@ -1549,133 +1552,7 @@
     <t>intervention_funding_total</t>
   </si>
   <si>
-    <t>Number of ntational staff in IMST</t>
-  </si>
-  <si>
-    <t>BLANK</t>
-  </si>
-  <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Adding duplicate for misspelt english version</t>
-  </si>
-  <si>
-    <t>Number of points of entry with  screening, isolation facilities and referral system for COVID-19</t>
-  </si>
-  <si>
-    <t>Number of contacts identified during the last 7 days</t>
-  </si>
-  <si>
-    <t>Total number of contacts under follow-up during the last 7 day</t>
-  </si>
-  <si>
-    <t>Total number of contacts under follow-up</t>
-  </si>
-  <si>
-    <t>Number of laboratory results made available within 48 hours for samples collected within the last two days</t>
-  </si>
-  <si>
-    <t>Performance Indicator 17: Bed occupancy rate for confirmed cases at present</t>
-  </si>
-  <si>
-    <t>Estimate of percentageof individuals reached by RCCE activity (e.g. CHW  trainings, health worker trainings, hotline usage )</t>
-  </si>
-  <si>
-    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the last month</t>
-  </si>
-  <si>
-    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the same month in 2019</t>
-  </si>
-  <si>
-    <t>Number of people living with HIV in target area who received ART in the current week</t>
-  </si>
-  <si>
-    <t>Total number of contacts under follow-up during the last 7 days</t>
-  </si>
-  <si>
-    <t>Total approved national COVID-19 response budget ($)</t>
-  </si>
-  <si>
-    <t>Amount of approved budget national budget utilized to date ($)</t>
-  </si>
-  <si>
-    <t>Total WCO response funding ($)</t>
-  </si>
-  <si>
-    <t>Amount of WCO response funding utilized to date ($)</t>
-  </si>
-  <si>
-    <t>Anticipated total IMST staff needed</t>
-  </si>
-  <si>
-    <t>Nuimber of points of entry with  screening, isolation facilities and referral system for COVID-19</t>
-  </si>
-  <si>
-    <t>Cumulative number of tests per 10 000 population performed at the end of the previous week  ( Tests-3501)</t>
-  </si>
-  <si>
-    <t>Cumulative number of tests per 10 000 population performed at the end of the current week  (Tests-2071)</t>
-  </si>
-  <si>
-    <t>Number of consultations in primary health facilities and prenatal clinics during the same month in 2019 (August)</t>
-  </si>
-  <si>
-    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the last month  (August 2020)</t>
-  </si>
-  <si>
-    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the same month (August 2019)</t>
-  </si>
-  <si>
-    <t>Number of people living with HIV in target area who received ART in the current week (Annual  total for 2020)</t>
-  </si>
-  <si>
-    <t>Number of people living with HIV in target area who received ART during the same week in 2019 (Annual total for 2019)</t>
-  </si>
-  <si>
-    <t>Cumulative number of tests per 10 000 population performed at the end of the previous week  ( Tests-1633) =1633/13785346.5</t>
-  </si>
-  <si>
-    <t>Cumulative number of tests per 10 000 population performed at the end of the current week  (Tests-2024)=2024/13785346.5</t>
-  </si>
-  <si>
-    <t>Number of consultations in primary health facilities and prenatal clinics during the last month (September 2020)</t>
-  </si>
-  <si>
-    <t>Number of consultations in primary health facilities and prenatal clinics during the same month in 2019 (September)</t>
-  </si>
-  <si>
-    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the last month  (Sept 2020)</t>
-  </si>
-  <si>
-    <t>Number of surviving infants receivig third dose of DPT-containing vaccine during the same month (Sept 2019)</t>
-  </si>
-  <si>
-    <t>Nombre de cas contacts signalés au cours des sept derniers jours</t>
-  </si>
-  <si>
-    <t>Adding duplicate for misspelt french version</t>
-  </si>
-  <si>
-    <t>Nombre de cas contacts signalés ayant fait l’objet d’une investigation dans les 24 heures au cours des sept derniers jours</t>
-  </si>
-  <si>
-    <t>Indicateur d’exécution n° 5 : Pourcentage du personnel de l’ESGI du bureau de pays déployé dans les ESGI décentralisées ou les soutenant</t>
-  </si>
-  <si>
-    <t>Indicateur d’exécution n° 15 : Taux d’occupation actuel des lits par les cas suspects (en pourcentage)</t>
-  </si>
-  <si>
-    <t>Indicateur d’exécution n° 19 : Taux de létalité</t>
-  </si>
-  <si>
-    <t>Indicateur d’exécution n° 23 : Taux de létalité des cas confirmés signalés au cours des sept derniers jours</t>
-  </si>
-  <si>
-    <t>Nombre de patients en soins ambulatoires au cours du mois dernier ( Avril)</t>
-  </si>
-  <si>
-    <t>Adding duplicate misspelt french version</t>
   </si>
 </sst>
 </file>
@@ -2027,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B134" sqref="B134"/>
+    <sheetView topLeftCell="A71" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,7 +1929,7 @@
         <v>356</v>
       </c>
       <c r="D1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2101,2140 +1978,1629 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B6" t="s">
-        <v>510</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>524</v>
-      </c>
-      <c r="D6" t="s">
-        <v>512</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>211</v>
+        <v>507</v>
       </c>
       <c r="B8" t="s">
-        <v>510</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>525</v>
-      </c>
-      <c r="D8" t="s">
-        <v>512</v>
+        <v>363</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>508</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>507</v>
+        <v>213</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>507</v>
+        <v>214</v>
       </c>
       <c r="B11" t="s">
-        <v>510</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>526</v>
-      </c>
-      <c r="D11" t="s">
-        <v>512</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>508</v>
+        <v>215</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>508</v>
+        <v>216</v>
       </c>
       <c r="B13" t="s">
-        <v>510</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>527</v>
-      </c>
-      <c r="D13" t="s">
-        <v>512</v>
+        <v>368</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>215</v>
-      </c>
-      <c r="B17" t="s">
-        <v>510</v>
+        <v>220</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="C17" t="s">
-        <v>528</v>
-      </c>
-      <c r="D17" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="B20" t="s">
-        <v>510</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>509</v>
-      </c>
-      <c r="D20" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>220</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>199</v>
+        <v>226</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>220</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>546</v>
+        <v>227</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>510</v>
-      </c>
-      <c r="D24" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>225</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C35" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="B36" t="s">
-        <v>510</v>
+        <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>513</v>
-      </c>
-      <c r="D36" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B37" t="s">
-        <v>510</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>529</v>
-      </c>
-      <c r="D37" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>240</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="B50" t="s">
-        <v>543</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>510</v>
-      </c>
-      <c r="D50" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="B52" t="s">
-        <v>545</v>
+        <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>510</v>
-      </c>
-      <c r="D52" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="B55" t="s">
-        <v>510</v>
+        <v>55</v>
       </c>
       <c r="C55" t="s">
-        <v>514</v>
-      </c>
-      <c r="D55" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="B57" t="s">
-        <v>510</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>515</v>
-      </c>
-      <c r="D57" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>246</v>
+        <v>260</v>
       </c>
       <c r="B58" t="s">
-        <v>510</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>247</v>
+        <v>261</v>
       </c>
       <c r="B59" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C59" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="B60" t="s">
-        <v>510</v>
+        <v>60</v>
       </c>
       <c r="C60" t="s">
-        <v>516</v>
-      </c>
-      <c r="D60" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>248</v>
-      </c>
-      <c r="B61" t="s">
-        <v>46</v>
+        <v>263</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="C61" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="B62" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>250</v>
-      </c>
-      <c r="B63" t="s">
-        <v>48</v>
+        <v>265</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="C63" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="B64" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="B65" t="s">
-        <v>510</v>
+        <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>517</v>
-      </c>
-      <c r="D65" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="B66" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="B67" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="B68" t="s">
-        <v>510</v>
+        <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>530</v>
-      </c>
-      <c r="D68" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="B69" t="s">
-        <v>510</v>
+        <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>254</v>
-      </c>
-      <c r="B71" t="s">
-        <v>510</v>
+        <v>273</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="C71" t="s">
-        <v>531</v>
-      </c>
-      <c r="D71" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>254</v>
+        <v>274</v>
       </c>
       <c r="B72" t="s">
-        <v>510</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>256</v>
+        <v>276</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="C75" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="B76" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C76" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="B77" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="B78" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="B79" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C79" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="B80" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C80" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C81" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>263</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>547</v>
+        <v>284</v>
+      </c>
+      <c r="B82" t="s">
+        <v>78</v>
       </c>
       <c r="C82" t="s">
-        <v>510</v>
-      </c>
-      <c r="D82" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="B83" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C83" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>265</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>174</v>
+        <v>286</v>
+      </c>
+      <c r="B84" t="s">
+        <v>80</v>
       </c>
       <c r="C84" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="B85" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C85" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="B86" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C86" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>268</v>
+        <v>289</v>
       </c>
       <c r="B87" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C87" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="B88" t="s">
-        <v>510</v>
+        <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>518</v>
-      </c>
-      <c r="D88" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>269</v>
+        <v>291</v>
       </c>
       <c r="B89" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C89" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="B90" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C90" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="B91" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C91" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="B92" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="C92" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>273</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>170</v>
+        <v>295</v>
+      </c>
+      <c r="B93" t="s">
+        <v>89</v>
       </c>
       <c r="C93" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>273</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>548</v>
+        <v>296</v>
+      </c>
+      <c r="B94" t="s">
+        <v>90</v>
       </c>
       <c r="C94" t="s">
-        <v>510</v>
-      </c>
-      <c r="D94" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="B95" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="B96" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="B97" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C97" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="B98" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="C98" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="B99" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="C99" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="B100" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="C100" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="B101" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="C101" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="B102" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="C102" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="B103" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="C103" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>283</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>162</v>
+        <v>306</v>
+      </c>
+      <c r="B104" t="s">
+        <v>100</v>
       </c>
       <c r="C104" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>283</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>549</v>
+        <v>307</v>
+      </c>
+      <c r="B105" t="s">
+        <v>101</v>
       </c>
       <c r="C105" t="s">
-        <v>510</v>
-      </c>
-      <c r="D105" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="B106" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="C106" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>285</v>
+        <v>309</v>
       </c>
       <c r="B107" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>286</v>
+        <v>310</v>
       </c>
       <c r="B108" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="C108" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>287</v>
+        <v>311</v>
       </c>
       <c r="B109" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
       <c r="B110" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="C110" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
       <c r="B111" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>290</v>
+        <v>314</v>
       </c>
       <c r="B112" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="B113" t="s">
-        <v>510</v>
+        <v>109</v>
       </c>
       <c r="C113" t="s">
-        <v>519</v>
-      </c>
-      <c r="D113" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>291</v>
+        <v>316</v>
       </c>
       <c r="B114" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C114" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>292</v>
+        <v>317</v>
       </c>
       <c r="B115" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="C115" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>293</v>
+        <v>318</v>
       </c>
       <c r="B116" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="C116" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>294</v>
+        <v>319</v>
       </c>
       <c r="B117" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
       <c r="C117" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="B118" t="s">
-        <v>89</v>
+        <v>114</v>
       </c>
       <c r="C118" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c r="B119" t="s">
-        <v>510</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s">
-        <v>539</v>
-      </c>
-      <c r="D119" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="B120" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="C120" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>296</v>
+        <v>323</v>
       </c>
       <c r="B121" t="s">
-        <v>510</v>
+        <v>117</v>
       </c>
       <c r="C121" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>296</v>
+        <v>324</v>
       </c>
       <c r="B122" t="s">
-        <v>510</v>
+        <v>118</v>
       </c>
       <c r="C122" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="B123" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="C123" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>298</v>
+        <v>326</v>
       </c>
       <c r="B124" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="C124" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>298</v>
+        <v>327</v>
       </c>
       <c r="B125" t="s">
-        <v>510</v>
+        <v>121</v>
       </c>
       <c r="C125" t="s">
-        <v>520</v>
-      </c>
-      <c r="D125" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>298</v>
+        <v>328</v>
       </c>
       <c r="B126" t="s">
-        <v>510</v>
+        <v>122</v>
       </c>
       <c r="C126" t="s">
-        <v>533</v>
-      </c>
-      <c r="D126" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>298</v>
+        <v>329</v>
       </c>
       <c r="B127" t="s">
-        <v>510</v>
+        <v>123</v>
       </c>
       <c r="C127" t="s">
-        <v>541</v>
-      </c>
-      <c r="D127" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>299</v>
+        <v>330</v>
       </c>
       <c r="B128" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="C128" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
       <c r="B129" t="s">
-        <v>510</v>
+        <v>125</v>
       </c>
       <c r="C129" t="s">
-        <v>521</v>
-      </c>
-      <c r="D129" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>299</v>
+        <v>332</v>
       </c>
       <c r="B130" t="s">
-        <v>510</v>
+        <v>126</v>
       </c>
       <c r="C130" t="s">
-        <v>534</v>
-      </c>
-      <c r="D130" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
       <c r="B131" t="s">
-        <v>510</v>
+        <v>127</v>
       </c>
       <c r="C131" t="s">
-        <v>542</v>
-      </c>
-      <c r="D131" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="B132" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C132" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>301</v>
+        <v>335</v>
       </c>
       <c r="B133" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="C133" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>301</v>
+        <v>336</v>
       </c>
       <c r="B134" t="s">
-        <v>550</v>
+        <v>130</v>
       </c>
       <c r="C134" t="s">
-        <v>510</v>
-      </c>
-      <c r="D134" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>302</v>
+        <v>337</v>
       </c>
       <c r="B135" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="C135" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>303</v>
+        <v>338</v>
       </c>
       <c r="B136" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="C136" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>304</v>
+        <v>339</v>
       </c>
       <c r="B137" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C137" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>304</v>
+        <v>340</v>
       </c>
       <c r="B138" t="s">
-        <v>510</v>
+        <v>134</v>
       </c>
       <c r="C138" t="s">
-        <v>522</v>
-      </c>
-      <c r="D138" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>304</v>
+        <v>341</v>
       </c>
       <c r="B139" t="s">
-        <v>510</v>
+        <v>135</v>
       </c>
       <c r="C139" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>305</v>
+        <v>342</v>
       </c>
       <c r="B140" t="s">
-        <v>99</v>
+        <v>136</v>
       </c>
       <c r="C140" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>305</v>
+        <v>343</v>
       </c>
       <c r="B141" t="s">
-        <v>510</v>
+        <v>137</v>
       </c>
       <c r="C141" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>306</v>
+        <v>344</v>
       </c>
       <c r="B142" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="C142" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>307</v>
+        <v>345</v>
       </c>
       <c r="B143" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="C143" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>308</v>
+        <v>346</v>
       </c>
       <c r="B144" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C144" t="s">
-        <v>461</v>
+        <v>140</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>309</v>
+        <v>347</v>
       </c>
       <c r="B145" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="C145" t="s">
-        <v>462</v>
+        <v>141</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>310</v>
+        <v>348</v>
       </c>
       <c r="B146" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="C146" t="s">
-        <v>463</v>
+        <v>142</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>311</v>
+        <v>349</v>
       </c>
       <c r="B147" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="C147" t="s">
-        <v>464</v>
+        <v>143</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>312</v>
+        <v>350</v>
       </c>
       <c r="B148" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="C148" t="s">
-        <v>465</v>
+        <v>144</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>313</v>
+        <v>351</v>
       </c>
       <c r="B149" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="C149" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>314</v>
+        <v>352</v>
       </c>
       <c r="B150" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="C150" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>315</v>
+        <v>353</v>
       </c>
       <c r="B151" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
       <c r="C151" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>316</v>
+        <v>354</v>
       </c>
       <c r="B152" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="C152" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>317</v>
+        <v>355</v>
       </c>
       <c r="B153" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="C153" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>318</v>
-      </c>
-      <c r="B154" t="s">
-        <v>112</v>
-      </c>
-      <c r="C154" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>319</v>
-      </c>
-      <c r="B155" t="s">
-        <v>113</v>
-      </c>
-      <c r="C155" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>320</v>
-      </c>
-      <c r="B156" t="s">
-        <v>114</v>
-      </c>
-      <c r="C156" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>321</v>
-      </c>
-      <c r="B157" t="s">
-        <v>115</v>
-      </c>
-      <c r="C157" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>322</v>
-      </c>
-      <c r="B158" t="s">
-        <v>116</v>
-      </c>
-      <c r="C158" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>323</v>
-      </c>
-      <c r="B159" t="s">
-        <v>117</v>
-      </c>
-      <c r="C159" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>324</v>
-      </c>
-      <c r="B160" t="s">
-        <v>118</v>
-      </c>
-      <c r="C160" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>325</v>
-      </c>
-      <c r="B161" t="s">
-        <v>119</v>
-      </c>
-      <c r="C161" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>326</v>
-      </c>
-      <c r="B162" t="s">
-        <v>120</v>
-      </c>
-      <c r="C162" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>327</v>
-      </c>
-      <c r="B163" t="s">
-        <v>121</v>
-      </c>
-      <c r="C163" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>328</v>
-      </c>
-      <c r="B164" t="s">
-        <v>122</v>
-      </c>
-      <c r="C164" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>329</v>
-      </c>
-      <c r="B165" t="s">
-        <v>123</v>
-      </c>
-      <c r="C165" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>330</v>
-      </c>
-      <c r="B166" t="s">
-        <v>124</v>
-      </c>
-      <c r="C166" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>331</v>
-      </c>
-      <c r="B167" t="s">
-        <v>125</v>
-      </c>
-      <c r="C167" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>332</v>
-      </c>
-      <c r="B168" t="s">
-        <v>126</v>
-      </c>
-      <c r="C168" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>333</v>
-      </c>
-      <c r="B169" t="s">
-        <v>127</v>
-      </c>
-      <c r="C169" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>334</v>
-      </c>
-      <c r="B170" t="s">
-        <v>128</v>
-      </c>
-      <c r="C170" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>335</v>
-      </c>
-      <c r="B171" t="s">
-        <v>129</v>
-      </c>
-      <c r="C171" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>336</v>
-      </c>
-      <c r="B172" t="s">
-        <v>130</v>
-      </c>
-      <c r="C172" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>337</v>
-      </c>
-      <c r="B173" t="s">
-        <v>131</v>
-      </c>
-      <c r="C173" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>338</v>
-      </c>
-      <c r="B174" t="s">
-        <v>132</v>
-      </c>
-      <c r="C174" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>339</v>
-      </c>
-      <c r="B175" t="s">
-        <v>133</v>
-      </c>
-      <c r="C175" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>340</v>
-      </c>
-      <c r="B176" t="s">
-        <v>134</v>
-      </c>
-      <c r="C176" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>341</v>
-      </c>
-      <c r="B177" t="s">
-        <v>135</v>
-      </c>
-      <c r="C177" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>342</v>
-      </c>
-      <c r="B178" t="s">
-        <v>136</v>
-      </c>
-      <c r="C178" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>343</v>
-      </c>
-      <c r="B179" t="s">
-        <v>137</v>
-      </c>
-      <c r="C179" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>344</v>
-      </c>
-      <c r="B180" t="s">
-        <v>138</v>
-      </c>
-      <c r="C180" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>345</v>
-      </c>
-      <c r="B181" t="s">
-        <v>139</v>
-      </c>
-      <c r="C181" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>346</v>
-      </c>
-      <c r="B182" t="s">
-        <v>140</v>
-      </c>
-      <c r="C182" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>347</v>
-      </c>
-      <c r="B183" t="s">
-        <v>141</v>
-      </c>
-      <c r="C183" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>348</v>
-      </c>
-      <c r="B184" t="s">
-        <v>142</v>
-      </c>
-      <c r="C184" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>349</v>
-      </c>
-      <c r="B185" t="s">
-        <v>143</v>
-      </c>
-      <c r="C185" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>350</v>
-      </c>
-      <c r="B186" t="s">
-        <v>144</v>
-      </c>
-      <c r="C186" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>351</v>
-      </c>
-      <c r="B187" t="s">
-        <v>145</v>
-      </c>
-      <c r="C187" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A188" t="s">
-        <v>352</v>
-      </c>
-      <c r="B188" t="s">
-        <v>146</v>
-      </c>
-      <c r="C188" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A189" t="s">
-        <v>353</v>
-      </c>
-      <c r="B189" t="s">
-        <v>147</v>
-      </c>
-      <c r="C189" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A190" t="s">
-        <v>354</v>
-      </c>
-      <c r="B190" t="s">
-        <v>148</v>
-      </c>
-      <c r="C190" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>355</v>
-      </c>
-      <c r="B191" t="s">
-        <v>149</v>
-      </c>
-      <c r="C191" t="s">
         <v>149</v>
       </c>
     </row>
@@ -4248,8 +3614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add grps to dict and update merge fn
</commit_message>
<xml_diff>
--- a/inst/extdata/mne_dictionary.xlsx
+++ b/inst/extdata/mne_dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="743">
   <si>
     <t>var_name</t>
   </si>
@@ -2241,6 +2241,18 @@
   </si>
   <si>
     <t>obs_vars</t>
+  </si>
+  <si>
+    <t>grp_type</t>
+  </si>
+  <si>
+    <t>Identifiers</t>
+  </si>
+  <si>
+    <t>Submitted documents</t>
+  </si>
+  <si>
+    <t>Observations</t>
   </si>
 </sst>
 </file>
@@ -2626,11 +2638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E24" sqref="E24"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2640,9 +2652,10 @@
     <col min="3" max="3" width="85.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2658,8 +2671,11 @@
       <c r="E1" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -2672,8 +2688,11 @@
       <c r="E2" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>208</v>
       </c>
@@ -2686,8 +2705,11 @@
       <c r="E3" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>209</v>
       </c>
@@ -2700,8 +2722,11 @@
       <c r="E4" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>210</v>
       </c>
@@ -2714,8 +2739,11 @@
       <c r="E5" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -2728,8 +2756,11 @@
       <c r="E6" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -2742,8 +2773,11 @@
       <c r="E7" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>507</v>
       </c>
@@ -2756,8 +2790,11 @@
       <c r="E8" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>508</v>
       </c>
@@ -2770,8 +2807,11 @@
       <c r="E9" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>213</v>
       </c>
@@ -2784,8 +2824,11 @@
       <c r="E10" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>214</v>
       </c>
@@ -2798,8 +2841,11 @@
       <c r="E11" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>215</v>
       </c>
@@ -2812,8 +2858,11 @@
       <c r="E12" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>216</v>
       </c>
@@ -2826,8 +2875,11 @@
       <c r="E13" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>217</v>
       </c>
@@ -2840,8 +2892,11 @@
       <c r="E14" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>218</v>
       </c>
@@ -2854,8 +2909,11 @@
       <c r="E15" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>219</v>
       </c>
@@ -2868,8 +2926,11 @@
       <c r="E16" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>220</v>
       </c>
@@ -2882,8 +2943,11 @@
       <c r="E17" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>221</v>
       </c>
@@ -2896,8 +2960,11 @@
       <c r="E18" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -2910,8 +2977,11 @@
       <c r="E19" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -2924,8 +2994,11 @@
       <c r="E20" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -2938,8 +3011,11 @@
       <c r="E21" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -2952,8 +3028,11 @@
       <c r="E22" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -2966,8 +3045,11 @@
       <c r="E23" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>227</v>
       </c>
@@ -2980,8 +3062,11 @@
       <c r="E24" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>228</v>
       </c>
@@ -2994,8 +3079,11 @@
       <c r="E25" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>229</v>
       </c>
@@ -3008,8 +3096,11 @@
       <c r="E26" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>230</v>
       </c>
@@ -3022,8 +3113,11 @@
       <c r="E27" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>231</v>
       </c>
@@ -3036,8 +3130,11 @@
       <c r="E28" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -3050,8 +3147,11 @@
       <c r="E29" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>232</v>
       </c>
@@ -3064,8 +3164,11 @@
       <c r="E30" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>233</v>
       </c>
@@ -3078,8 +3181,11 @@
       <c r="E31" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>234</v>
       </c>
@@ -3092,8 +3198,11 @@
       <c r="E32" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>235</v>
       </c>
@@ -3106,8 +3215,11 @@
       <c r="E33" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>236</v>
       </c>
@@ -3120,8 +3232,11 @@
       <c r="E34" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>237</v>
       </c>
@@ -3134,8 +3249,11 @@
       <c r="E35" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>238</v>
       </c>
@@ -3148,8 +3266,11 @@
       <c r="E36" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>239</v>
       </c>
@@ -3162,8 +3283,11 @@
       <c r="E37" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>240</v>
       </c>
@@ -3176,8 +3300,11 @@
       <c r="E38" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>241</v>
       </c>
@@ -3190,8 +3317,11 @@
       <c r="E39" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>242</v>
       </c>
@@ -3204,8 +3334,11 @@
       <c r="E40" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>243</v>
       </c>
@@ -3218,8 +3351,11 @@
       <c r="E41" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>244</v>
       </c>
@@ -3232,8 +3368,11 @@
       <c r="E42" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>245</v>
       </c>
@@ -3246,8 +3385,11 @@
       <c r="E43" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>246</v>
       </c>
@@ -3260,8 +3402,11 @@
       <c r="E44" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>247</v>
       </c>
@@ -3274,8 +3419,11 @@
       <c r="E45" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>248</v>
       </c>
@@ -3288,8 +3436,11 @@
       <c r="E46" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>249</v>
       </c>
@@ -3302,8 +3453,11 @@
       <c r="E47" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>250</v>
       </c>
@@ -3316,8 +3470,11 @@
       <c r="E48" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>251</v>
       </c>
@@ -3330,8 +3487,11 @@
       <c r="E49" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>252</v>
       </c>
@@ -3344,8 +3504,11 @@
       <c r="E50" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>253</v>
       </c>
@@ -3358,8 +3521,11 @@
       <c r="E51" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>254</v>
       </c>
@@ -3372,8 +3538,11 @@
       <c r="E52" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>255</v>
       </c>
@@ -3386,8 +3555,11 @@
       <c r="E53" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>256</v>
       </c>
@@ -3400,8 +3572,11 @@
       <c r="E54" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>257</v>
       </c>
@@ -3414,8 +3589,11 @@
       <c r="E55" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>258</v>
       </c>
@@ -3428,8 +3606,11 @@
       <c r="E56" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>259</v>
       </c>
@@ -3442,8 +3623,11 @@
       <c r="E57" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>260</v>
       </c>
@@ -3456,8 +3640,11 @@
       <c r="E58" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>261</v>
       </c>
@@ -3470,8 +3657,11 @@
       <c r="E59" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>262</v>
       </c>
@@ -3484,8 +3674,11 @@
       <c r="E60" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>263</v>
       </c>
@@ -3498,8 +3691,11 @@
       <c r="E61" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>264</v>
       </c>
@@ -3512,8 +3708,11 @@
       <c r="E62" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>265</v>
       </c>
@@ -3526,8 +3725,11 @@
       <c r="E63" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>266</v>
       </c>
@@ -3540,8 +3742,11 @@
       <c r="E64" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>267</v>
       </c>
@@ -3554,8 +3759,11 @@
       <c r="E65" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>268</v>
       </c>
@@ -3568,8 +3776,11 @@
       <c r="E66" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>269</v>
       </c>
@@ -3582,8 +3793,11 @@
       <c r="E67" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>270</v>
       </c>
@@ -3596,8 +3810,11 @@
       <c r="E68" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>271</v>
       </c>
@@ -3610,8 +3827,11 @@
       <c r="E69" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>272</v>
       </c>
@@ -3624,8 +3844,11 @@
       <c r="E70" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>273</v>
       </c>
@@ -3638,8 +3861,11 @@
       <c r="E71" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>274</v>
       </c>
@@ -3652,8 +3878,11 @@
       <c r="E72" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>275</v>
       </c>
@@ -3666,8 +3895,11 @@
       <c r="E73" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>276</v>
       </c>
@@ -3680,8 +3912,11 @@
       <c r="E74" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>277</v>
       </c>
@@ -3694,8 +3929,11 @@
       <c r="E75" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>278</v>
       </c>
@@ -3708,8 +3946,11 @@
       <c r="E76" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>279</v>
       </c>
@@ -3722,8 +3963,11 @@
       <c r="E77" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>280</v>
       </c>
@@ -3736,8 +3980,11 @@
       <c r="E78" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>281</v>
       </c>
@@ -3750,8 +3997,11 @@
       <c r="E79" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>282</v>
       </c>
@@ -3764,8 +4014,11 @@
       <c r="E80" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>283</v>
       </c>
@@ -3778,8 +4031,11 @@
       <c r="E81" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>284</v>
       </c>
@@ -3792,8 +4048,11 @@
       <c r="E82" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>285</v>
       </c>
@@ -3806,8 +4065,11 @@
       <c r="E83" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>286</v>
       </c>
@@ -3820,8 +4082,11 @@
       <c r="E84" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>287</v>
       </c>
@@ -3834,8 +4099,11 @@
       <c r="E85" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>288</v>
       </c>
@@ -3848,8 +4116,11 @@
       <c r="E86" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>289</v>
       </c>
@@ -3862,8 +4133,11 @@
       <c r="E87" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>290</v>
       </c>
@@ -3876,8 +4150,11 @@
       <c r="E88" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>291</v>
       </c>
@@ -3890,8 +4167,11 @@
       <c r="E89" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>292</v>
       </c>
@@ -3904,8 +4184,11 @@
       <c r="E90" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>293</v>
       </c>
@@ -3918,8 +4201,11 @@
       <c r="E91" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>294</v>
       </c>
@@ -3932,8 +4218,11 @@
       <c r="E92" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>295</v>
       </c>
@@ -3946,8 +4235,11 @@
       <c r="E93" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>296</v>
       </c>
@@ -3960,8 +4252,11 @@
       <c r="E94" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>297</v>
       </c>
@@ -3974,8 +4269,11 @@
       <c r="E95" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>298</v>
       </c>
@@ -3988,8 +4286,11 @@
       <c r="E96" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>299</v>
       </c>
@@ -4002,8 +4303,11 @@
       <c r="E97" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>300</v>
       </c>
@@ -4016,8 +4320,11 @@
       <c r="E98" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>301</v>
       </c>
@@ -4030,8 +4337,11 @@
       <c r="E99" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>302</v>
       </c>
@@ -4044,8 +4354,11 @@
       <c r="E100" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>303</v>
       </c>
@@ -4058,8 +4371,11 @@
       <c r="E101" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>304</v>
       </c>
@@ -4072,8 +4388,11 @@
       <c r="E102" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F102" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>305</v>
       </c>
@@ -4086,8 +4405,11 @@
       <c r="E103" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>306</v>
       </c>
@@ -4100,8 +4422,11 @@
       <c r="E104" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F104" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>307</v>
       </c>
@@ -4114,8 +4439,11 @@
       <c r="E105" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F105" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>308</v>
       </c>
@@ -4128,8 +4456,11 @@
       <c r="E106" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>309</v>
       </c>
@@ -4142,8 +4473,11 @@
       <c r="E107" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>310</v>
       </c>
@@ -4156,8 +4490,11 @@
       <c r="E108" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>311</v>
       </c>
@@ -4170,8 +4507,11 @@
       <c r="E109" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>312</v>
       </c>
@@ -4184,8 +4524,11 @@
       <c r="E110" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>313</v>
       </c>
@@ -4198,8 +4541,11 @@
       <c r="E111" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>314</v>
       </c>
@@ -4212,8 +4558,11 @@
       <c r="E112" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>315</v>
       </c>
@@ -4226,8 +4575,11 @@
       <c r="E113" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>316</v>
       </c>
@@ -4240,8 +4592,11 @@
       <c r="E114" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>317</v>
       </c>
@@ -4254,8 +4609,11 @@
       <c r="E115" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F115" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>318</v>
       </c>
@@ -4268,8 +4626,11 @@
       <c r="E116" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F116" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>319</v>
       </c>
@@ -4282,8 +4643,11 @@
       <c r="E117" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F117" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>320</v>
       </c>
@@ -4296,8 +4660,11 @@
       <c r="E118" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F118" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>321</v>
       </c>
@@ -4310,8 +4677,11 @@
       <c r="E119" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F119" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>322</v>
       </c>
@@ -4324,8 +4694,11 @@
       <c r="E120" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F120" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>323</v>
       </c>
@@ -4338,8 +4711,11 @@
       <c r="E121" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F121" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>324</v>
       </c>
@@ -4352,8 +4728,11 @@
       <c r="E122" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>325</v>
       </c>
@@ -4366,8 +4745,11 @@
       <c r="E123" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F123" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>326</v>
       </c>
@@ -4380,8 +4762,11 @@
       <c r="E124" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F124" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>327</v>
       </c>
@@ -4394,8 +4779,11 @@
       <c r="E125" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F125" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>328</v>
       </c>
@@ -4408,8 +4796,11 @@
       <c r="E126" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F126" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>329</v>
       </c>
@@ -4422,8 +4813,11 @@
       <c r="E127" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F127" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>330</v>
       </c>
@@ -4436,8 +4830,11 @@
       <c r="E128" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F128" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>331</v>
       </c>
@@ -4450,8 +4847,11 @@
       <c r="E129" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F129" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>332</v>
       </c>
@@ -4464,8 +4864,11 @@
       <c r="E130" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F130" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>333</v>
       </c>
@@ -4478,8 +4881,11 @@
       <c r="E131" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F131" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>334</v>
       </c>
@@ -4492,8 +4898,11 @@
       <c r="E132" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F132" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>335</v>
       </c>
@@ -4506,8 +4915,11 @@
       <c r="E133" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F133" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>336</v>
       </c>
@@ -4520,8 +4932,11 @@
       <c r="E134" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F134" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>337</v>
       </c>
@@ -4534,8 +4949,11 @@
       <c r="E135" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F135" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>338</v>
       </c>
@@ -4548,8 +4966,11 @@
       <c r="E136" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F136" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>339</v>
       </c>
@@ -4562,8 +4983,11 @@
       <c r="E137" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F137" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>340</v>
       </c>
@@ -4576,8 +5000,11 @@
       <c r="E138" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F138" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>341</v>
       </c>
@@ -4590,8 +5017,11 @@
       <c r="E139" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F139" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>342</v>
       </c>
@@ -4604,8 +5034,11 @@
       <c r="E140" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F140" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>343</v>
       </c>
@@ -4618,8 +5051,11 @@
       <c r="E141" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F141" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>344</v>
       </c>
@@ -4632,8 +5068,11 @@
       <c r="E142" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F142" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>345</v>
       </c>
@@ -4646,8 +5085,11 @@
       <c r="E143" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F143" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>346</v>
       </c>
@@ -4660,8 +5102,11 @@
       <c r="E144" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F144" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>347</v>
       </c>
@@ -4674,8 +5119,11 @@
       <c r="E145" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F145" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>348</v>
       </c>
@@ -4688,8 +5136,11 @@
       <c r="E146" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F146" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>349</v>
       </c>
@@ -4702,8 +5153,11 @@
       <c r="E147" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F147" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>350</v>
       </c>
@@ -4716,8 +5170,11 @@
       <c r="E148" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F148" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>351</v>
       </c>
@@ -4730,8 +5187,11 @@
       <c r="E149" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F149" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>352</v>
       </c>
@@ -4744,8 +5204,11 @@
       <c r="E150" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F150" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>353</v>
       </c>
@@ -4758,8 +5221,11 @@
       <c r="E151" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F151" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>354</v>
       </c>
@@ -4772,8 +5238,11 @@
       <c r="E152" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F152" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>355</v>
       </c>
@@ -4785,6 +5254,9 @@
       </c>
       <c r="E153" t="s">
         <v>738</v>
+      </c>
+      <c r="F153" t="s">
+        <v>742</v>
       </c>
     </row>
   </sheetData>
@@ -4798,7 +5270,7 @@
   <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>